<commit_message>
Dinesh[Enh] - Added Selenium Notes Excel into Directory
</commit_message>
<xml_diff>
--- a/TestExcels/Test_Details.xlsx
+++ b/TestExcels/Test_Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Selenium\1. nC\nC_Selenium\TestExcels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F68EB3C-6DD6-421D-A514-183AA7848E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AC4564-CDAE-4CF9-9DAE-5F4BD3524DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="614" xr2:uid="{77C8A981-06A5-485C-861C-4A0B52044819}"/>
   </bookViews>
@@ -598,7 +598,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,7 +632,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>10</v>

</xml_diff>